<commit_message>
Add HttpBrowser analyzer skeletton + resouces refactor
</commit_message>
<xml_diff>
--- a/docs/BugHunter-checkList.xlsx
+++ b/docs/BugHunter-checkList.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="79">
   <si>
     <t>Description</t>
   </si>
@@ -250,13 +250,22 @@
   </si>
   <si>
     <t xml:space="preserve">split ot separate code fixes </t>
+  </si>
+  <si>
+    <t>BH1006</t>
+  </si>
+  <si>
+    <t>BH1007</t>
+  </si>
+  <si>
+    <t>need to check for Request.Browser.Browser</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -276,6 +285,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -313,7 +330,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -323,6 +340,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
     <fill>
@@ -379,27 +401,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="2"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="3"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Input" xfId="2" builtinId="20"/>
+    <cellStyle name="Input" xfId="3" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -715,7 +740,7 @@
   <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -978,31 +1003,49 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B14" s="10" t="s">
+    <row r="14" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B14" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E14" t="b">
-        <v>1</v>
-      </c>
-      <c r="K14" t="s">
+      <c r="E14" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F14" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G14" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H14" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="K14" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B15" s="10" t="s">
+    <row r="15" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E15" t="b">
-        <v>1</v>
-      </c>
-      <c r="K15" t="s">
+      <c r="D15" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="E15" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="K15" s="11" t="s">
         <v>42</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Split HttpRequestAndResponseCookies into two.
BugHunter now contains two separate analyzers, code fixes and tests
one for Request and one for Response cookies.
</commit_message>
<xml_diff>
--- a/docs/BugHunter-checkList.xlsx
+++ b/docs/BugHunter-checkList.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6810"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="86">
   <si>
     <t>Description</t>
   </si>
@@ -138,9 +138,6 @@
     <t>Request.UserHostAddress property is used. Use RequestContext.UserHostAddress instead.</t>
   </si>
   <si>
-    <t>Cookies (request+response)</t>
-  </si>
-  <si>
     <t>Request.Url is used. Use RequestContext.Url instead.</t>
   </si>
   <si>
@@ -192,9 +189,6 @@
     <t>FormsAuthentication.SignOut is used directly. Use AuthenticationHelper.SignOut instead.</t>
   </si>
   <si>
-    <t xml:space="preserve"> BH1002</t>
-  </si>
-  <si>
     <t>Note</t>
   </si>
   <si>
@@ -213,9 +207,6 @@
     <t>BH1004</t>
   </si>
   <si>
-    <t>HttpSessionElementAccess</t>
-  </si>
-  <si>
     <t>Analyzer name</t>
   </si>
   <si>
@@ -240,18 +231,9 @@
     <t>WhereLikeMethod</t>
   </si>
   <si>
-    <t>RequestUserHostAddress</t>
-  </si>
-  <si>
     <t>BH1005</t>
   </si>
   <si>
-    <t>HttpRequestAndResponseCookies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">split ot separate code fixes </t>
-  </si>
-  <si>
     <t>BH1006</t>
   </si>
   <si>
@@ -259,18 +241,65 @@
   </si>
   <si>
     <t>need to check for Request.Browser.Browser</t>
+  </si>
+  <si>
+    <t>BH10X1</t>
+  </si>
+  <si>
+    <t>BH10X2</t>
+  </si>
+  <si>
+    <t>HttpSessionElementAccessGet</t>
+  </si>
+  <si>
+    <t>HttpSessionElementAccessSet</t>
+  </si>
+  <si>
+    <t>BH1002</t>
+  </si>
+  <si>
+    <t>HttpRequestCookies</t>
+  </si>
+  <si>
+    <t>HttpResponseCookies</t>
+  </si>
+  <si>
+    <t>Cookies</t>
+  </si>
+  <si>
+    <t>BH10XX</t>
+  </si>
+  <si>
+    <t>HttpRequestUrl</t>
+  </si>
+  <si>
+    <t>HttpRequestBrowser</t>
+  </si>
+  <si>
+    <t>HttpRequestUserHostAddress</t>
+  </si>
+  <si>
+    <t>HttpResponseRedirect</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -292,33 +321,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C5700"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -327,10 +340,20 @@
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -344,12 +367,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
@@ -401,31 +431,40 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="3"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="4">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Input" xfId="3" builtinId="20"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="5">
+    <cellStyle name="20 % - zvýraznenie5" xfId="3" builtinId="46"/>
+    <cellStyle name="60 % - zvýraznenie5" xfId="4" builtinId="48"/>
+    <cellStyle name="Dobrá" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutrálna" xfId="2" builtinId="28"/>
+    <cellStyle name="Normálna" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -737,39 +776,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M28"/>
+  <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="35" style="10" customWidth="1"/>
+    <col min="1" max="1" width="12.25" style="3" customWidth="1"/>
+    <col min="2" max="2" width="35" style="1" customWidth="1"/>
     <col min="3" max="3" width="27" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="4" max="4" width="35.125" customWidth="1"/>
     <col min="5" max="5" width="27" customWidth="1"/>
-    <col min="6" max="8" width="13.28515625" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" customWidth="1"/>
-    <col min="12" max="12" width="18.7109375" customWidth="1"/>
-    <col min="13" max="13" width="17.5703125" customWidth="1"/>
+    <col min="6" max="8" width="13.25" customWidth="1"/>
+    <col min="9" max="9" width="13.125" customWidth="1"/>
+    <col min="10" max="10" width="14.125" customWidth="1"/>
+    <col min="11" max="11" width="14.875" customWidth="1"/>
+    <col min="12" max="12" width="18.75" customWidth="1"/>
+    <col min="13" max="13" width="17.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>64</v>
+      <c r="B1" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>33</v>
@@ -781,7 +820,7 @@
         <v>32</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>3</v>
@@ -800,124 +839,196 @@
       </c>
     </row>
     <row r="2" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="F2" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="G2" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H2" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>27</v>
-      </c>
+      <c r="B2" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="A3" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D4" t="s">
-        <v>68</v>
-      </c>
+      <c r="A4" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
     </row>
     <row r="5" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="9" t="s">
+      <c r="A5" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="G5" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H5" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F8" t="b">
-        <v>1</v>
-      </c>
-      <c r="G8" t="b">
-        <v>1</v>
-      </c>
-      <c r="H8" t="b">
-        <v>1</v>
-      </c>
+      <c r="B8" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G8" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
       <c r="K8" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B9" s="9" t="s">
+      <c r="A9" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>72</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>10</v>
       </c>
       <c r="E9" s="4" t="b">
         <v>1</v>
@@ -927,309 +1038,373 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="10" t="s">
+      <c r="A10" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="F10" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="G10" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="H10" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="I10" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="J10" s="14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="G11" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="H11" s="10" t="b">
+        <v>1</v>
+      </c>
+      <c r="K11" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="F12" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13"/>
+      <c r="E13"/>
+      <c r="F13"/>
+      <c r="G13"/>
+      <c r="H13"/>
+      <c r="I13"/>
+      <c r="J13"/>
+    </row>
+    <row r="14" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+      <c r="B14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14"/>
+      <c r="F14"/>
+      <c r="G14"/>
+      <c r="H14"/>
+      <c r="I14"/>
+      <c r="J14"/>
+    </row>
+    <row r="15" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15"/>
+      <c r="E15"/>
+      <c r="F15"/>
+      <c r="G15"/>
+      <c r="H15"/>
+      <c r="I15"/>
+      <c r="J15"/>
+      <c r="K15" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16"/>
+      <c r="F16"/>
+      <c r="G16"/>
+      <c r="H16"/>
+      <c r="I16"/>
+      <c r="J16"/>
+      <c r="K16" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="B17" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17"/>
+      <c r="E17" t="b">
+        <v>1</v>
+      </c>
+      <c r="F17" t="b">
+        <v>1</v>
+      </c>
+      <c r="G17" t="b">
+        <v>1</v>
+      </c>
+      <c r="H17" t="b">
+        <v>1</v>
+      </c>
+      <c r="I17"/>
+      <c r="J17"/>
+      <c r="K17" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C18" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="E11" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="K11" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E12" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="F12" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="G12" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H12" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E13" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="F13" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="G13" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H13" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="K13" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="F14" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="G14" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H14" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="K14" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="E15" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="K15" s="11" t="s">
+      <c r="K18" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B16" s="10" t="s">
+    <row r="19" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="B19" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E16" t="b">
-        <v>1</v>
-      </c>
-      <c r="K16" t="s">
+      <c r="D19"/>
+      <c r="E19" t="b">
+        <v>1</v>
+      </c>
+      <c r="F19"/>
+      <c r="G19"/>
+      <c r="H19"/>
+      <c r="I19"/>
+      <c r="J19"/>
+      <c r="K19" s="7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" t="b">
-        <v>1</v>
-      </c>
-      <c r="G17" t="s">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" t="s">
         <v>45</v>
       </c>
-      <c r="K17" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="E21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B22" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B23" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" t="s">
         <v>47</v>
-      </c>
-      <c r="E19" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E20" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D22" t="s">
-        <v>48</v>
-      </c>
-      <c r="E22" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D23" t="s">
-        <v>49</v>
-      </c>
-      <c r="E23" t="b">
-        <v>0</v>
-      </c>
-      <c r="K23" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D24" t="s">
-        <v>59</v>
       </c>
       <c r="E24" t="b">
         <v>0</v>
       </c>
-      <c r="K24" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B25" s="10" t="s">
-        <v>22</v>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
+      </c>
+      <c r="D25" t="s">
+        <v>48</v>
       </c>
       <c r="E25" t="b">
         <v>0</v>
       </c>
       <c r="K25" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B26" s="10" t="s">
-        <v>53</v>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>53</v>
+        <v>21</v>
+      </c>
+      <c r="D26" t="s">
+        <v>57</v>
       </c>
       <c r="E26" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B27" s="10" t="s">
+      <c r="K26" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27" t="b">
+        <v>0</v>
+      </c>
+      <c r="K27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B29" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C29" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E27" t="b">
-        <v>1</v>
-      </c>
-      <c r="K27" t="s">
+      <c r="E29" t="b">
+        <v>1</v>
+      </c>
+      <c r="K29" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B30" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E30" t="b">
+        <v>1</v>
+      </c>
+      <c r="K30" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B28" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E28" t="b">
-        <v>1</v>
-      </c>
-      <c r="K28" t="s">
-        <v>55</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:J1"/>
+  <autoFilter ref="A1:J1">
+    <sortState ref="A2:J30">
+      <sortCondition ref="A1"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Add analyzer for ClientScript, not complete
It will probably need to be changed, and look for method invocation.
Tests are commented out and codefix does not work yet.
</commit_message>
<xml_diff>
--- a/docs/BugHunter-checkList.xlsx
+++ b/docs/BugHunter-checkList.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="93">
   <si>
     <t>Description</t>
   </si>
@@ -162,9 +162,6 @@
     <t>uf, uf, uf</t>
   </si>
   <si>
-    <t>many, many cases</t>
-  </si>
-  <si>
     <t xml:space="preserve"> --&gt; ??</t>
   </si>
   <si>
@@ -289,6 +286,21 @@
   </si>
   <si>
     <t>BH1010</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>PagePostBack</t>
+  </si>
+  <si>
+    <t>PageCallback</t>
+  </si>
+  <si>
+    <t>what should be the first argument?</t>
+  </si>
+  <si>
+    <t>BH011</t>
   </si>
 </sst>
 </file>
@@ -447,7 +459,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -457,16 +469,15 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="4" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="20 % - zvýraznenie5" xfId="3" builtinId="46"/>
@@ -787,8 +798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -811,13 +822,13 @@
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>62</v>
-      </c>
       <c r="D1" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>33</v>
@@ -829,7 +840,7 @@
         <v>32</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>3</v>
@@ -848,40 +859,40 @@
       </c>
     </row>
     <row r="2" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="F2" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="G2" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="H2" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
+      <c r="B2" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>35</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4" t="b">
@@ -901,13 +912,13 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4" t="b">
@@ -926,89 +937,89 @@
       <c r="J4" s="4"/>
     </row>
     <row r="5" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B6" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="C5" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="F5" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="G5" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="H5" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="B6" s="16" t="s">
+      <c r="C6" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="C6" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="F6" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="G6" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="H6" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="C7" s="14" t="s">
+      <c r="A7" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="F7" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="G7" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="H7" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>12</v>
@@ -1034,16 +1045,16 @@
     </row>
     <row r="9" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E9" s="4" t="b">
         <v>1</v>
@@ -1053,134 +1064,136 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+    </row>
+    <row r="11" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="K11" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="K12" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="F13" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G13" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H13" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="J13" s="13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="B10" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="F10" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="G10" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="H10" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="I10" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="J10" s="14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="C11" s="10" t="s">
+      <c r="B14" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="G11" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="H11" s="10" t="b">
-        <v>1</v>
-      </c>
-      <c r="K11" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="C12" s="9" t="s">
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G14" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H14" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+    </row>
+    <row r="15" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C15" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="F12" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="G12" s="9" t="s">
+      <c r="D15" s="16"/>
+      <c r="E15" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F15" s="16" t="b">
+        <v>1</v>
+      </c>
+      <c r="G15" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13"/>
-      <c r="E13"/>
-      <c r="F13"/>
-      <c r="G13"/>
-      <c r="H13"/>
-      <c r="I13"/>
-      <c r="J13"/>
-    </row>
-    <row r="14" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D14" t="s">
-        <v>65</v>
-      </c>
-      <c r="E14"/>
-      <c r="F14"/>
-      <c r="G14"/>
-      <c r="H14"/>
-      <c r="I14"/>
-      <c r="J14"/>
-    </row>
-    <row r="15" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15"/>
-      <c r="E15"/>
-      <c r="F15"/>
-      <c r="G15"/>
-      <c r="H15"/>
-      <c r="I15"/>
-      <c r="J15"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="16"/>
       <c r="K15" s="4" t="s">
         <v>40</v>
       </c>
@@ -1188,14 +1201,12 @@
     <row r="16" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" t="s">
-        <v>56</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D16"/>
       <c r="E16"/>
       <c r="F16"/>
       <c r="G16"/>
@@ -1208,25 +1219,19 @@
     </row>
     <row r="17" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
-      <c r="B17" s="11" t="s">
-        <v>9</v>
+      <c r="B17" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17"/>
-      <c r="E17" t="b">
-        <v>1</v>
-      </c>
-      <c r="F17" t="b">
-        <v>1</v>
-      </c>
-      <c r="G17" t="b">
-        <v>1</v>
-      </c>
-      <c r="H17" t="b">
-        <v>1</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="D17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E17"/>
+      <c r="F17"/>
+      <c r="G17"/>
+      <c r="H17"/>
       <c r="I17"/>
       <c r="J17"/>
       <c r="K17" s="4" t="s">
@@ -1235,10 +1240,10 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="K18" t="s">
         <v>42</v>
@@ -1247,15 +1252,15 @@
     <row r="19" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D19"/>
-      <c r="E19" t="b">
-        <v>1</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="D19" t="s">
+        <v>55</v>
+      </c>
+      <c r="E19"/>
       <c r="F19"/>
       <c r="G19"/>
       <c r="H19"/>
@@ -1266,161 +1271,183 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" t="b">
+        <v>1</v>
+      </c>
+      <c r="F20" t="b">
+        <v>1</v>
+      </c>
+      <c r="G20" t="b">
+        <v>1</v>
+      </c>
+      <c r="H20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22"/>
+      <c r="E22" t="b">
+        <v>1</v>
+      </c>
+      <c r="F22"/>
+      <c r="G22"/>
+      <c r="H22"/>
+      <c r="I22"/>
+      <c r="J22"/>
+    </row>
+    <row r="23" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+      <c r="B23" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C23" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D23" t="s">
         <v>45</v>
       </c>
-      <c r="F20" s="3"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="13" t="s">
+      <c r="E23"/>
+      <c r="F23" s="3"/>
+      <c r="G23"/>
+      <c r="H23"/>
+      <c r="I23"/>
+      <c r="J23"/>
+    </row>
+    <row r="24" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B24" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C24" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D21" t="s">
-        <v>46</v>
-      </c>
-      <c r="E21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E22" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E23" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D24" t="s">
-        <v>47</v>
-      </c>
-      <c r="E24" t="b">
-        <v>0</v>
+      <c r="D24" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="E24" s="7" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D25" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E25" t="b">
         <v>0</v>
       </c>
       <c r="K25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D26" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="E26" t="b">
         <v>0</v>
       </c>
       <c r="K26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="D27" t="s">
+        <v>56</v>
       </c>
       <c r="E27" t="b">
         <v>0</v>
       </c>
       <c r="K27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="E28" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B29" s="13" t="s">
+      <c r="B29" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E29" t="b">
+        <v>0</v>
+      </c>
+      <c r="K29" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="3"/>
+      <c r="B30" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C30" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E29" t="b">
-        <v>1</v>
-      </c>
-      <c r="K29" t="s">
+      <c r="D30" t="s">
+        <v>88</v>
+      </c>
+      <c r="E30" t="b">
+        <v>1</v>
+      </c>
+      <c r="F30"/>
+      <c r="G30"/>
+      <c r="H30"/>
+      <c r="I30"/>
+      <c r="J30"/>
+      <c r="K30" s="4" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E30" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="K30" s="4" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add StringManipulationMethods analyzer, codefix and tests
</commit_message>
<xml_diff>
--- a/docs/BugHunter-checkList.xlsx
+++ b/docs/BugHunter-checkList.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17426"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6810"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="97">
   <si>
     <t>Description</t>
   </si>
@@ -258,9 +258,6 @@
     <t>BH1008</t>
   </si>
   <si>
-    <t>BH10XX</t>
-  </si>
-  <si>
     <t>HttpRequestUrl</t>
   </si>
   <si>
@@ -279,18 +276,12 @@
     <t>BH1010</t>
   </si>
   <si>
-    <t>???</t>
-  </si>
-  <si>
     <t>PagePostBack</t>
   </si>
   <si>
     <t>PageCallback</t>
   </si>
   <si>
-    <t>BH011</t>
-  </si>
-  <si>
     <t>ma sa volat s invariant culture alebo inym modifikatorom</t>
   </si>
   <si>
@@ -310,13 +301,25 @@
   </si>
   <si>
     <t>Consistency that it always is CMS.XY[.Internal]</t>
+  </si>
+  <si>
+    <t>BH10X3</t>
+  </si>
+  <si>
+    <t>BH1011</t>
+  </si>
+  <si>
+    <t>BH1012</t>
+  </si>
+  <si>
+    <t>Qualified vs Identifier name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -374,9 +377,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF9C5700"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -384,10 +386,18 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -410,12 +420,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
       </patternFill>
@@ -423,6 +427,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
       </patternFill>
     </fill>
   </fills>
@@ -479,10 +488,10 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -493,23 +502,24 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="20 % - zvýraznenie5" xfId="3" builtinId="46"/>
-    <cellStyle name="60 % - zvýraznenie5" xfId="4" builtinId="48"/>
-    <cellStyle name="Dobrá" xfId="1" builtinId="26"/>
-    <cellStyle name="Neutrálna" xfId="2" builtinId="28"/>
-    <cellStyle name="Normálna" xfId="0" builtinId="0"/>
-    <cellStyle name="Zlá" xfId="5" builtinId="27"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Bad" xfId="4" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Input" xfId="5" builtinId="20"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -823,26 +833,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.26953125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" style="3" customWidth="1"/>
     <col min="2" max="2" width="35" style="1" customWidth="1"/>
     <col min="3" max="3" width="27" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.90625" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" customWidth="1"/>
     <col min="5" max="5" width="27" customWidth="1"/>
-    <col min="6" max="8" width="13.26953125" customWidth="1"/>
-    <col min="9" max="9" width="13.08984375" customWidth="1"/>
-    <col min="10" max="10" width="14.08984375" customWidth="1"/>
-    <col min="11" max="11" width="14.90625" customWidth="1"/>
-    <col min="12" max="12" width="18.7265625" customWidth="1"/>
-    <col min="13" max="13" width="17.6328125" customWidth="1"/>
+    <col min="6" max="8" width="13.28515625" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" customWidth="1"/>
+    <col min="12" max="12" width="18.7109375" customWidth="1"/>
+    <col min="13" max="13" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
@@ -883,33 +893,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="15" t="s">
+    <row r="2" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F2" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G2" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H2" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D2" s="12"/>
+      <c r="E2" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>35</v>
       </c>
@@ -935,7 +945,7 @@
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>73</v>
       </c>
@@ -961,90 +971,90 @@
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
     </row>
-    <row r="5" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="13" t="s">
+    <row r="5" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F5" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G5" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H5" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A6" s="13" t="s">
+      <c r="D5" s="12"/>
+      <c r="E5" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F6" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G6" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H6" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A7" s="15" t="s">
+      <c r="D6" s="12"/>
+      <c r="E6" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="B7" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C7" s="13" t="s">
+      <c r="B7" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F7" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G7" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H7" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D7" s="12"/>
+      <c r="E7" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>66</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>12</v>
@@ -1068,12 +1078,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>67</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>13</v>
@@ -1088,32 +1098,32 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-    </row>
-    <row r="11" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D10" s="12"/>
+      <c r="E10" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+    </row>
+    <row r="11" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>18</v>
@@ -1125,12 +1135,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>29</v>
@@ -1142,148 +1152,148 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="15" t="s">
+    <row r="13" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E13" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B14" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C14" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13" t="b">
+      <c r="D14" s="12"/>
+      <c r="E14" s="12" t="b">
         <v>0</v>
       </c>
-      <c r="F13" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G13" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H13" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="I13" s="13" t="s">
+      <c r="F14" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G14" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H14" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="I14" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="J13" s="13" t="s">
+      <c r="J14" s="12" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="15" t="s">
+    <row r="15" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B15" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C15" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G14" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H14" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-    </row>
-    <row r="15" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="F15" s="16" t="b">
-        <v>1</v>
-      </c>
-      <c r="G15" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G15" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H15" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
       <c r="K15" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="3"/>
-      <c r="B16" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16"/>
-      <c r="E16"/>
-      <c r="F16"/>
-      <c r="G16"/>
-      <c r="H16"/>
-      <c r="I16"/>
-      <c r="J16"/>
-      <c r="K16" s="4" t="s">
+    <row r="16" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="E16" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="K16" s="7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="3"/>
-      <c r="B17" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D17" t="s">
-        <v>61</v>
-      </c>
-      <c r="E17"/>
-      <c r="F17"/>
-      <c r="G17"/>
-      <c r="H17"/>
-      <c r="I17"/>
-      <c r="J17"/>
+    <row r="17" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="F17" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
       <c r="K17" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="K18" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
-      <c r="B19" s="1" t="s">
-        <v>8</v>
+      <c r="B19" s="15" t="s">
+        <v>6</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" t="s">
-        <v>53</v>
+        <v>60</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>61</v>
       </c>
       <c r="E19"/>
       <c r="F19"/>
@@ -1295,113 +1305,107 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B20" s="10" t="s">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C22" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="E20" t="b">
-        <v>1</v>
-      </c>
-      <c r="F20" t="b">
-        <v>1</v>
-      </c>
-      <c r="G20" t="b">
-        <v>1</v>
-      </c>
-      <c r="H20" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B21" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="3"/>
-      <c r="B22" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>14</v>
       </c>
       <c r="D22"/>
       <c r="E22" t="b">
         <v>1</v>
       </c>
-      <c r="F22"/>
-      <c r="G22"/>
-      <c r="H22"/>
+      <c r="F22" t="b">
+        <v>1</v>
+      </c>
+      <c r="G22" t="b">
+        <v>1</v>
+      </c>
+      <c r="H22" t="b">
+        <v>1</v>
+      </c>
       <c r="I22"/>
       <c r="J22"/>
     </row>
-    <row r="23" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D23" t="s">
-        <v>89</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="D23"/>
       <c r="E23"/>
-      <c r="F23" s="3"/>
+      <c r="F23"/>
       <c r="G23"/>
       <c r="H23"/>
       <c r="I23"/>
       <c r="J23"/>
     </row>
-    <row r="24" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="E24" s="7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B25" s="18" t="s">
-        <v>19</v>
+    <row r="24" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3"/>
+      <c r="B24" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24"/>
+      <c r="E24" t="b">
+        <v>1</v>
+      </c>
+      <c r="F24"/>
+      <c r="G24"/>
+      <c r="H24"/>
+      <c r="I24"/>
+      <c r="J24"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D25" t="s">
-        <v>90</v>
-      </c>
-      <c r="E25" t="b">
-        <v>0</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="F25" s="3"/>
       <c r="K25" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B26" s="18" t="s">
-        <v>20</v>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B26" s="15" t="s">
+        <v>19</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D26" t="s">
-        <v>45</v>
+        <v>87</v>
       </c>
       <c r="E26" t="b">
         <v>0</v>
@@ -1410,15 +1414,15 @@
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B27" s="1" t="s">
-        <v>21</v>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B27" s="15" t="s">
+        <v>20</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D27" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="E27" t="b">
         <v>0</v>
@@ -1427,26 +1431,29 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B28" s="18" t="s">
-        <v>22</v>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D28" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E28" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B29" s="18" t="s">
-        <v>49</v>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B29" s="15" t="s">
+        <v>22</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>49</v>
+        <v>22</v>
+      </c>
+      <c r="D29" t="s">
+        <v>88</v>
       </c>
       <c r="E29" t="b">
         <v>0</v>
@@ -1455,19 +1462,17 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
-      <c r="B30" s="12" t="s">
-        <v>23</v>
+      <c r="B30" s="15" t="s">
+        <v>49</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D30" t="s">
-        <v>85</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="D30"/>
       <c r="E30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F30"/>
       <c r="G30"/>
@@ -1478,17 +1483,17 @@
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:J1">
-    <sortState ref="A2:J30">
+    <sortState ref="A2:J31">
       <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
Update checklist and RunChurnTest woth correct commit
</commit_message>
<xml_diff>
--- a/docs/BugHunter-checkList.xlsx
+++ b/docs/BugHunter-checkList.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6810"/>
@@ -10,7 +10,7 @@
     <sheet name="CsChecks" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CsChecks!$A$1:$J$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CsChecks!$A$1:$J$36</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -252,12 +252,6 @@
     <t>meno triedy v nom</t>
   </si>
   <si>
-    <t xml:space="preserve">Namespaces </t>
-  </si>
-  <si>
-    <t>Consistency that it always is CMS.XY[.Internal]</t>
-  </si>
-  <si>
     <t>BH10X3</t>
   </si>
   <si>
@@ -291,9 +285,6 @@
     <t>BH2005</t>
   </si>
   <si>
-    <t>BH2006</t>
-  </si>
-  <si>
     <t>StringCompareToMethod</t>
   </si>
   <si>
@@ -306,16 +297,25 @@
     <t>StringCompareStaticMethod</t>
   </si>
   <si>
-    <t>StringEqualsStaticMethod</t>
-  </si>
-  <si>
     <t>introduce variable when needed (preceding member access)</t>
+  </si>
+  <si>
+    <t>BH3000</t>
+  </si>
+  <si>
+    <t>some performance refactoring more than welcome</t>
+  </si>
+  <si>
+    <t>BH4000</t>
+  </si>
+  <si>
+    <t>WP - ValidationHelperGet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -495,10 +495,10 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="3" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Bad" xfId="3" builtinId="27"/>
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Dobrá" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutrálna" xfId="2" builtinId="28"/>
+    <cellStyle name="Normálna" xfId="0" builtinId="0"/>
+    <cellStyle name="Zlá" xfId="3" builtinId="27"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -810,10 +810,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M37"/>
+  <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1132,7 +1132,7 @@
     </row>
     <row r="14" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B14" s="13" t="s">
         <v>67</v>
@@ -1156,7 +1156,7 @@
     </row>
     <row r="15" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B15" s="12" t="s">
         <v>9</v>
@@ -1233,7 +1233,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B18" s="12" t="s">
         <v>23</v>
@@ -1253,10 +1253,10 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>16</v>
@@ -1271,10 +1271,10 @@
     </row>
     <row r="20" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>16</v>
@@ -1282,16 +1282,16 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>16</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
@@ -1302,10 +1302,10 @@
     </row>
     <row r="22" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>16</v>
@@ -1313,10 +1313,10 @@
     </row>
     <row r="23" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>16</v>
@@ -1324,10 +1324,10 @@
     </row>
     <row r="24" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>16</v>
@@ -1335,34 +1335,45 @@
     </row>
     <row r="25" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="B25" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="B26" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B26" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
     </row>
     <row r="27" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
-      <c r="B27" s="17" t="s">
-        <v>6</v>
+      <c r="B27" s="16" t="s">
+        <v>5</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D27" t="s">
-        <v>48</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D27"/>
       <c r="E27"/>
       <c r="F27"/>
       <c r="G27"/>
@@ -1372,13 +1383,15 @@
     </row>
     <row r="28" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
-      <c r="B28" s="16" t="s">
-        <v>7</v>
+      <c r="B28" s="17" t="s">
+        <v>6</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D28"/>
+        <v>47</v>
+      </c>
+      <c r="D28" t="s">
+        <v>48</v>
+      </c>
       <c r="E28"/>
       <c r="F28"/>
       <c r="G28"/>
@@ -1389,14 +1402,12 @@
     <row r="29" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D29" t="s">
-        <v>40</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="D29"/>
       <c r="E29"/>
       <c r="F29"/>
       <c r="G29"/>
@@ -1404,15 +1415,17 @@
       <c r="I29"/>
       <c r="J29"/>
     </row>
-    <row r="30" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="16" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D30"/>
+        <v>8</v>
+      </c>
+      <c r="D30" t="s">
+        <v>40</v>
+      </c>
       <c r="E30"/>
       <c r="F30"/>
       <c r="G30"/>
@@ -1420,23 +1433,16 @@
       <c r="I30"/>
       <c r="J30"/>
     </row>
-    <row r="31" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="3"/>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B31" s="17" t="s">
         <v>14</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D31"/>
       <c r="E31" t="b">
         <v>1</v>
       </c>
-      <c r="F31"/>
-      <c r="G31"/>
-      <c r="H31"/>
-      <c r="I31"/>
-      <c r="J31"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B32" s="17" t="s">
@@ -1480,7 +1486,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="3"/>
       <c r="B35" s="17" t="s">
         <v>22</v>
       </c>
@@ -1493,6 +1500,11 @@
       <c r="E35" t="b">
         <v>0</v>
       </c>
+      <c r="F35"/>
+      <c r="G35"/>
+      <c r="H35"/>
+      <c r="I35"/>
+      <c r="J35"/>
     </row>
     <row r="36" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
@@ -1512,18 +1524,10 @@
       <c r="I36"/>
       <c r="J36"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B37" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:J37">
-    <sortState ref="A2:J37">
-      <sortCondition ref="A1:A37"/>
+  <autoFilter ref="A1:J36">
+    <sortState ref="A2:J36">
+      <sortCondition ref="A1:A36"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update checklists with all not yet implemented BH checks
</commit_message>
<xml_diff>
--- a/docs/BugHunter-checkList.xlsx
+++ b/docs/BugHunter-checkList.xlsx
@@ -10,7 +10,7 @@
     <sheet name="CsChecks" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CsChecks!$A$1:$J$36</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CsChecks!$A$1:$I$36</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -22,14 +22,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="119">
   <si>
     <t>Description</t>
   </si>
   <si>
-    <t>Is implemented</t>
-  </si>
-  <si>
     <t>Id</t>
   </si>
   <si>
@@ -147,9 +144,6 @@
     <t xml:space="preserve"> --&gt;AspxChecks?</t>
   </si>
   <si>
-    <t>Has tests</t>
-  </si>
-  <si>
     <t>BH1003</t>
   </si>
   <si>
@@ -310,13 +304,88 @@
   </si>
   <si>
     <t>WP - ValidationHelperGet</t>
+  </si>
+  <si>
+    <t>Folder</t>
+  </si>
+  <si>
+    <t>WpChecks</t>
+  </si>
+  <si>
+    <t>Aspx</t>
+  </si>
+  <si>
+    <t>CodeFile</t>
+  </si>
+  <si>
+    <t>Base</t>
+  </si>
+  <si>
+    <t>Methods</t>
+  </si>
+  <si>
+    <t>Preco to nie je riesene cez nejaky interface?</t>
+  </si>
+  <si>
+    <t>RelativePaths</t>
+  </si>
+  <si>
+    <t>Da sa na to pouzit roslyn? (vid prvy riadok, if endsWith .cs return)</t>
+  </si>
+  <si>
+    <t>PageChecks</t>
+  </si>
+  <si>
+    <t>XElementExtensionMethods</t>
+  </si>
+  <si>
+    <t>TryGetElementValue</t>
+  </si>
+  <si>
+    <t>IsUtilityProjectType</t>
+  </si>
+  <si>
+    <t>IsProjectTypeOf</t>
+  </si>
+  <si>
+    <t>ControlCheck</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>ReferenceExtensionMethods</t>
+  </si>
+  <si>
+    <t>VersionMatchHintPathVersion</t>
+  </si>
+  <si>
+    <t>ProjectCheck</t>
+  </si>
+  <si>
+    <t>DocumentationEnabled</t>
+  </si>
+  <si>
+    <t>GlobalAssemblyInfoLinked</t>
+  </si>
+  <si>
+    <t>CheckCmsDependencies</t>
+  </si>
+  <si>
+    <t>CheckCmsDependenciesDefault</t>
+  </si>
+  <si>
+    <t>CheckCmsDependenciesForWebApp</t>
+  </si>
+  <si>
+    <t>CheckOutputAndReferencedProjects</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -394,6 +463,15 @@
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -474,7 +552,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -493,6 +571,7 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Dobrá" xfId="1" builtinId="26"/>
@@ -810,362 +889,349 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M36"/>
+  <dimension ref="A1:L53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.28515625" style="3" customWidth="1"/>
     <col min="2" max="2" width="35" style="16" customWidth="1"/>
-    <col min="3" max="3" width="27" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" customWidth="1"/>
-    <col min="5" max="5" width="27" customWidth="1"/>
-    <col min="6" max="8" width="13.28515625" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" customWidth="1"/>
-    <col min="12" max="12" width="18.7109375" customWidth="1"/>
-    <col min="13" max="13" width="17.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" style="16" customWidth="1"/>
+    <col min="4" max="4" width="27" style="1" customWidth="1"/>
+    <col min="5" max="5" width="35.85546875" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" customWidth="1"/>
+    <col min="12" max="12" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>41</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>30</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="M1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9" t="b">
-        <v>1</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="9"/>
       <c r="F3" s="9" t="b">
         <v>1</v>
       </c>
       <c r="G3" s="9" t="b">
         <v>1</v>
       </c>
-      <c r="H3" s="9" t="b">
-        <v>1</v>
-      </c>
+      <c r="H3" s="9"/>
       <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+    </row>
+    <row r="5" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="F4" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="G4" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H4" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-    </row>
-    <row r="5" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="B5" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E5" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="F5" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="G5" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H5" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" s="13" t="s">
+      <c r="C7" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="E7" s="9"/>
+      <c r="F7" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="G8" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+    </row>
+    <row r="9" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="F6" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="G6" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="H6" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="F7" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="G7" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="H7" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="C9" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G9" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B8" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="F8" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="G8" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="H8" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-    </row>
-    <row r="9" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="C9" s="4" t="s">
+      <c r="B10" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="F9" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="G9" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H9" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="F10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4" t="b">
+        <v>1</v>
+      </c>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-    </row>
-    <row r="11" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" s="8" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="B12" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="8" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="B13" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="F13" s="9"/>
+      <c r="C13" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-    </row>
-    <row r="14" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9" t="b">
-        <v>1</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="9"/>
       <c r="F14" s="9" t="b">
         <v>1</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-    </row>
-    <row r="15" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="4" t="b">
-        <v>1</v>
+        <v>8</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="F15" s="4" t="b">
         <v>1</v>
@@ -1173,360 +1239,533 @@
       <c r="G15" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="H15" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9" t="b">
+        <v>49</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="F16" s="9" t="b">
-        <v>1</v>
-      </c>
       <c r="G16" s="9" t="b">
         <v>1</v>
       </c>
-      <c r="H16" s="9" t="b">
-        <v>1</v>
+      <c r="H16" s="9" t="s">
+        <v>27</v>
       </c>
       <c r="I16" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="J16" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" s="9"/>
+        <v>48</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>33</v>
+      </c>
       <c r="E17" s="9"/>
-      <c r="F17" s="9" t="b">
-        <v>1</v>
-      </c>
+      <c r="F17" s="9"/>
       <c r="G17" s="9" t="b">
         <v>1</v>
       </c>
-      <c r="H17" s="9" t="b">
-        <v>1</v>
-      </c>
+      <c r="H17" s="9"/>
       <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="F18" s="4"/>
+        <v>22</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4" t="b">
+        <v>1</v>
+      </c>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" s="4"/>
+        <v>78</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-    </row>
-    <row r="20" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="B20" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
-        <v>83</v>
-      </c>
       <c r="B21" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>16</v>
+        <v>85</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>27</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="E21" s="7"/>
+        <v>15</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>89</v>
+      </c>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-    </row>
-    <row r="22" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B24" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B23" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B24" s="12" t="s">
+      <c r="C24" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
+      <c r="B25" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="B25" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D25" s="4" t="s">
+      <c r="B26" s="18" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B26" s="4" t="s">
+      <c r="C26" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="C26" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D26" s="4"/>
+      <c r="D26" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
-      <c r="J26" s="4"/>
-    </row>
-    <row r="27" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D27"/>
+        <v>4</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>4</v>
+      </c>
       <c r="E27"/>
       <c r="F27"/>
       <c r="G27"/>
       <c r="H27"/>
       <c r="I27"/>
-      <c r="J27"/>
-    </row>
-    <row r="28" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D28" t="s">
-        <v>48</v>
-      </c>
-      <c r="E28"/>
+        <v>5</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E28" t="s">
+        <v>46</v>
+      </c>
       <c r="F28"/>
       <c r="G28"/>
       <c r="H28"/>
       <c r="I28"/>
-      <c r="J28"/>
-    </row>
-    <row r="29" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D29"/>
+        <v>6</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="E29"/>
       <c r="F29"/>
       <c r="G29"/>
       <c r="H29"/>
       <c r="I29"/>
-      <c r="J29"/>
-    </row>
-    <row r="30" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D30" t="s">
-        <v>40</v>
-      </c>
-      <c r="E30"/>
+        <v>7</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" t="s">
+        <v>39</v>
+      </c>
       <c r="F30"/>
       <c r="G30"/>
       <c r="H30"/>
       <c r="I30"/>
-      <c r="J30"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B31" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E31" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F31" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B32" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E32" t="s">
+        <v>71</v>
+      </c>
+      <c r="F32" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B33" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C33" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D33" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E33" t="s">
+        <v>36</v>
+      </c>
+      <c r="F33" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B34" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E34" t="s">
         <v>73</v>
       </c>
-      <c r="E32" t="b">
+      <c r="F34" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B33" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D33" t="s">
-        <v>37</v>
-      </c>
-      <c r="E33" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B34" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D34" t="s">
-        <v>75</v>
-      </c>
-      <c r="E34" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D35" t="s">
-        <v>74</v>
-      </c>
-      <c r="E35" t="b">
+        <v>21</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E35" t="s">
+        <v>72</v>
+      </c>
+      <c r="F35" t="b">
         <v>0</v>
       </c>
-      <c r="F35"/>
       <c r="G35"/>
       <c r="H35"/>
       <c r="I35"/>
-      <c r="J35"/>
-    </row>
-    <row r="36" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D36"/>
-      <c r="E36" t="b">
+        <v>37</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E36"/>
+      <c r="F36" t="b">
         <v>0</v>
       </c>
-      <c r="F36"/>
       <c r="G36"/>
       <c r="H36"/>
       <c r="I36"/>
-      <c r="J36"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B37" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="C37" s="16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B38" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="C38" s="16" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B39" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="C39" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="E39" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B40" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="C40" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="E40" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B41" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="C41" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B42" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="C42" s="16" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B43" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="C43" s="16" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B44" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="C44" s="16" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B45" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="C45" s="16" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B46" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="C46" s="16" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B47" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="C47" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="E47" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B48" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="C48" s="16" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B49" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="C49" s="16" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B50" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="C50" s="16" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B51" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="C51" s="16" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B52" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="C52" s="16" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B53" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="C53" s="16" t="s">
+        <v>112</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J36">
-    <sortState ref="A2:J36">
+  <autoFilter ref="A1:I36">
+    <sortState ref="A2:I36">
       <sortCondition ref="A1:A36"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
Extend WebPartBase tests with fake filePaths
Specify diagnostic location of WpCheckBase
</commit_message>
<xml_diff>
--- a/docs/BugHunter-checkList.xlsx
+++ b/docs/BugHunter-checkList.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6810"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="138">
   <si>
     <t>Description</t>
   </si>
@@ -430,12 +430,18 @@
   </si>
   <si>
     <t>E</t>
+  </si>
+  <si>
+    <t>BH4001</t>
+  </si>
+  <si>
+    <t>WebPartBase</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -675,11 +681,11 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Bad" xfId="3" builtinId="27"/>
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="4" builtinId="10"/>
+    <cellStyle name="Dobrá" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutrálna" xfId="2" builtinId="28"/>
+    <cellStyle name="Normálna" xfId="0" builtinId="0"/>
+    <cellStyle name="Poznámka" xfId="4" builtinId="10"/>
+    <cellStyle name="Zlá" xfId="3" builtinId="27"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -994,7 +1000,7 @@
   <dimension ref="A1:L53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1053,20 +1059,24 @@
     </row>
     <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>95</v>
+        <v>137</v>
       </c>
       <c r="C2" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="D2" s="28"/>
+      <c r="D2" s="28" t="s">
+        <v>95</v>
+      </c>
       <c r="E2" s="28" t="s">
         <v>120</v>
       </c>
       <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
+      <c r="G2" s="28" t="b">
+        <v>0</v>
+      </c>
       <c r="H2" s="28"/>
       <c r="I2" s="28"/>
     </row>

</xml_diff>

<commit_message>
Introduce FakeFileInfo in tests
Previous solution where only the file path was possible to adjust was not
enough, since some analyzers are only applicable to documents with certain
file extensions. Therefore more configurable solution was needed.
</commit_message>
<xml_diff>
--- a/docs/BugHunter-checkList.xlsx
+++ b/docs/BugHunter-checkList.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="146">
   <si>
     <t>Description</t>
   </si>
@@ -457,6 +457,9 @@
   </si>
   <si>
     <t>BH10X4</t>
+  </si>
+  <si>
+    <t>ConnectionHelperExecuteQuery</t>
   </si>
 </sst>
 </file>
@@ -1026,7 +1029,7 @@
   <dimension ref="A1:L54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1109,7 +1112,7 @@
         <v>144</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>7</v>
+        <v>145</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
Set-up boilerpalete for BaseClass benchmarking
</commit_message>
<xml_diff>
--- a/docs/BugHunter-checkList.xlsx
+++ b/docs/BugHunter-checkList.xlsx
@@ -971,7 +971,7 @@
   <dimension ref="A1:G54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1387,7 +1387,9 @@
         <v>13</v>
       </c>
       <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
+      <c r="F20" s="6" t="b">
+        <v>1</v>
+      </c>
       <c r="G20" s="6"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1423,7 +1425,9 @@
         <v>2</v>
       </c>
       <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
+      <c r="F22" s="6" t="b">
+        <v>1</v>
+      </c>
       <c r="G22" s="6" t="s">
         <v>97</v>
       </c>
@@ -1444,7 +1448,9 @@
       <c r="E23" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="F23" s="6"/>
+      <c r="F23" s="8" t="b">
+        <v>1</v>
+      </c>
       <c r="G23" s="6"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1463,7 +1469,9 @@
       <c r="E24" s="6" t="b">
         <v>0</v>
       </c>
-      <c r="F24" s="6"/>
+      <c r="F24" s="8" t="b">
+        <v>1</v>
+      </c>
       <c r="G24" s="6"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1480,7 +1488,9 @@
         <v>79</v>
       </c>
       <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
+      <c r="F25" s="8" t="b">
+        <v>1</v>
+      </c>
       <c r="G25" s="3"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1497,7 +1507,9 @@
         <v>79</v>
       </c>
       <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
+      <c r="F26" s="8" t="b">
+        <v>1</v>
+      </c>
       <c r="G26" s="6"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>